<commit_message>
Diego Saavedra - Se modifica el modulo de Plantillas agregando la Plantilla Futbol 8 y Futbol 5 Empresas
</commit_message>
<xml_diff>
--- a/JCA_Futbol_Admin/Utiles/PlanillaFutbol5_Generada.xlsx
+++ b/JCA_Futbol_Admin/Utiles/PlanillaFutbol5_Generada.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
   <si>
     <t>PLANILLA OFICIAL</t>
   </si>
@@ -141,16 +141,16 @@
     <t>GOLES</t>
   </si>
   <si>
-    <t>Gustavo Adolfo Gonzalez</t>
+    <t>Jose Castillo</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Jose Gregorio Castillo</t>
+    <t>James Rodriguez</t>
   </si>
   <si>
-    <t>Diego Fernando Saavedra Reyes</t>
+    <t>Xabi Alonso</t>
   </si>
   <si>
     <t>DIRECTOR TECNICO</t>
@@ -177,13 +177,10 @@
     <t>2,PERIODO</t>
   </si>
   <si>
-    <t>Jaime Carreno</t>
+    <t>sebas melo</t>
   </si>
   <si>
-    <t>Carlos Agudelo</t>
-  </si>
-  <si>
-    <t>Sebastian Melo</t>
+    <t>gustaco de melo</t>
   </si>
   <si>
     <t>OFICIALES DE ARBITRAJE</t>
@@ -18237,7 +18234,9 @@
     </row>
     <row r="11" spans="1:16212" customHeight="1" ht="13.5">
       <c r="A11" s="1"/>
-      <c r="B11" s="131"/>
+      <c r="B11" s="131" t="s">
+        <v>4</v>
+      </c>
       <c r="C11" s="132"/>
       <c r="D11" s="132"/>
       <c r="E11" s="132"/>
@@ -18689,7 +18688,7 @@
     <row r="16" spans="1:16212" customHeight="1" ht="14.25">
       <c r="A16" s="1"/>
       <c r="B16" s="61">
-        <v>1234</v>
+        <v>6619</v>
       </c>
       <c r="C16" s="62"/>
       <c r="D16" s="62"/>
@@ -18783,7 +18782,7 @@
     <row r="17" spans="1:16212" customHeight="1" ht="14.25">
       <c r="A17" s="1"/>
       <c r="B17" s="61">
-        <v>123</v>
+        <v>1333</v>
       </c>
       <c r="C17" s="62"/>
       <c r="D17" s="62"/>
@@ -18868,7 +18867,7 @@
     <row r="18" spans="1:16212" customHeight="1" ht="14.25">
       <c r="A18" s="1"/>
       <c r="B18" s="61">
-        <v>1115854830</v>
+        <v>4567</v>
       </c>
       <c r="C18" s="62"/>
       <c r="D18" s="62"/>
@@ -20294,7 +20293,9 @@
     </row>
     <row r="36" spans="1:16212" customHeight="1" ht="13.5">
       <c r="A36" s="1"/>
-      <c r="B36" s="131"/>
+      <c r="B36" s="131" t="s">
+        <v>7</v>
+      </c>
       <c r="C36" s="132"/>
       <c r="D36" s="132"/>
       <c r="E36" s="132"/>
@@ -20746,7 +20747,7 @@
     <row r="41" spans="1:16212" customHeight="1" ht="14.25">
       <c r="A41" s="1"/>
       <c r="B41" s="61">
-        <v>222222</v>
+        <v>9234</v>
       </c>
       <c r="C41" s="62"/>
       <c r="D41" s="62"/>
@@ -20837,7 +20838,7 @@
     <row r="42" spans="1:16212" customHeight="1" ht="14.25">
       <c r="A42" s="1"/>
       <c r="B42" s="61">
-        <v>123456</v>
+        <v>3234</v>
       </c>
       <c r="C42" s="62"/>
       <c r="D42" s="62"/>
@@ -20921,16 +20922,12 @@
     </row>
     <row r="43" spans="1:16212" customHeight="1" ht="14.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="61">
-        <v>12345</v>
-      </c>
+      <c r="B43" s="61"/>
       <c r="C43" s="62"/>
       <c r="D43" s="62"/>
       <c r="E43" s="62"/>
       <c r="F43" s="63"/>
-      <c r="G43" s="93" t="s">
-        <v>55</v>
-      </c>
+      <c r="G43" s="93"/>
       <c r="H43" s="94"/>
       <c r="I43" s="94"/>
       <c r="J43" s="94"/>
@@ -22620,7 +22617,7 @@
     <row r="64" spans="1:16212" customHeight="1" ht="13.5">
       <c r="A64" s="1"/>
       <c r="B64" s="40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C64" s="40"/>
       <c r="D64" s="40"/>
@@ -22658,7 +22655,7 @@
       <c r="AJ64" s="40"/>
       <c r="AK64" s="40"/>
       <c r="AL64" s="40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AM64" s="40"/>
       <c r="AN64" s="40"/>
@@ -22675,7 +22672,7 @@
       <c r="AY64" s="40"/>
       <c r="AZ64" s="40"/>
       <c r="BA64" s="40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BB64" s="40"/>
       <c r="BC64" s="40"/>
@@ -22690,7 +22687,7 @@
       <c r="BL64" s="40"/>
       <c r="BM64" s="40"/>
       <c r="BN64" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="BO64" s="40"/>
       <c r="BP64" s="40"/>
@@ -22709,7 +22706,7 @@
     <row r="65" spans="1:16212" customHeight="1" ht="13.5">
       <c r="A65" s="1"/>
       <c r="B65" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C65" s="36"/>
       <c r="D65" s="36"/>
@@ -22762,20 +22759,20 @@
       <c r="AY65" s="35"/>
       <c r="AZ65" s="35"/>
       <c r="BA65" s="39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BB65" s="39"/>
       <c r="BC65" s="39"/>
       <c r="BD65" s="39"/>
       <c r="BE65" s="39"/>
       <c r="BF65" s="39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BG65" s="39"/>
       <c r="BH65" s="39"/>
       <c r="BI65" s="39"/>
       <c r="BJ65" s="39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BK65" s="39"/>
       <c r="BL65" s="39"/>
@@ -22802,7 +22799,7 @@
     <row r="66" spans="1:16212" customHeight="1" ht="13.5">
       <c r="A66" s="1"/>
       <c r="B66" s="36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C66" s="36"/>
       <c r="D66" s="36"/>
@@ -22855,7 +22852,7 @@
       <c r="AY66" s="35"/>
       <c r="AZ66" s="35"/>
       <c r="BA66" s="39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="BB66" s="39"/>
       <c r="BC66" s="39"/>
@@ -22891,7 +22888,7 @@
     <row r="67" spans="1:16212" customHeight="1" ht="13.5">
       <c r="A67" s="1"/>
       <c r="B67" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C67" s="36"/>
       <c r="D67" s="36"/>
@@ -22944,7 +22941,7 @@
       <c r="AY67" s="35"/>
       <c r="AZ67" s="35"/>
       <c r="BA67" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="BB67" s="39"/>
       <c r="BC67" s="39"/>
@@ -22959,7 +22956,7 @@
       <c r="BL67" s="39"/>
       <c r="BM67" s="39"/>
       <c r="BN67" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="BO67" s="39"/>
       <c r="BP67" s="39"/>
@@ -22980,7 +22977,7 @@
     <row r="68" spans="1:16212" customHeight="1" ht="13.5">
       <c r="A68" s="1"/>
       <c r="B68" s="36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C68" s="36"/>
       <c r="D68" s="36"/>
@@ -23033,7 +23030,7 @@
       <c r="AY68" s="35"/>
       <c r="AZ68" s="35"/>
       <c r="BA68" s="37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BB68" s="37"/>
       <c r="BC68" s="37"/>
@@ -23065,7 +23062,7 @@
     <row r="69" spans="1:16212" customHeight="1" ht="13.5">
       <c r="A69" s="1"/>
       <c r="B69" s="36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C69" s="36"/>
       <c r="D69" s="36"/>
@@ -23228,7 +23225,7 @@
     </row>
     <row r="71" spans="1:16212">
       <c r="B71" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C71" s="33"/>
       <c r="D71" s="33"/>
@@ -23240,7 +23237,7 @@
       <c r="J71" s="33"/>
       <c r="K71" s="33"/>
       <c r="L71" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M71" s="34"/>
       <c r="N71" s="34"/>

</xml_diff>